<commit_message>
comment id not publish to prod
</commit_message>
<xml_diff>
--- a/target/classes/data/data_test.xlsx
+++ b/target/classes/data/data_test.xlsx
@@ -9,38 +9,39 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7450"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7450" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login_Success" sheetId="15" r:id="rId1"/>
-    <sheet name="Edit_Profile_Input" sheetId="38" r:id="rId2"/>
-    <sheet name="Edit_Profile_Alert_Named" sheetId="40" r:id="rId3"/>
-    <sheet name="Edit_Profile_Validate_Button" sheetId="44" r:id="rId4"/>
-    <sheet name="Live_Tv_Active_Tab" sheetId="45" r:id="rId5"/>
-    <sheet name="Live_Tv_Tab_Live_And_Catch" sheetId="50" r:id="rId6"/>
-    <sheet name="Homepage_Menu_Tengah" sheetId="46" r:id="rId7"/>
-    <sheet name="Homepage_Menu_Bawah" sheetId="47" r:id="rId8"/>
-    <sheet name="Homepage_Menu_Bawah_Direct" sheetId="48" r:id="rId9"/>
-    <sheet name="Homepage_Menu_Tengah_Direct" sheetId="49" r:id="rId10"/>
-    <sheet name="Edit_Profile_Alert_Phone" sheetId="41" r:id="rId11"/>
-    <sheet name="List_Share" sheetId="35" r:id="rId12"/>
-    <sheet name="Login_Alert_Username" sheetId="20" r:id="rId13"/>
-    <sheet name="Login_Alert_Password" sheetId="21" r:id="rId14"/>
-    <sheet name="Login_Alert_Popup" sheetId="16" r:id="rId15"/>
-    <sheet name="List_Menu_Account_Popup_Login" sheetId="12" r:id="rId16"/>
-    <sheet name="List_Menu_Account_Direct" sheetId="11" r:id="rId17"/>
-    <sheet name="Register_Email_Alert" sheetId="22" r:id="rId18"/>
-    <sheet name="Register_Password1_Alert_Email" sheetId="23" r:id="rId19"/>
-    <sheet name="Register_Password2_Alert_Email" sheetId="24" r:id="rId20"/>
-    <sheet name="Register_Password2_Alert_Phone" sheetId="26" r:id="rId21"/>
-    <sheet name="Register_Password1_Alert_Phone" sheetId="27" r:id="rId22"/>
-    <sheet name="Register_Phone_Alert" sheetId="25" r:id="rId23"/>
-    <sheet name="Register_List_Gender" sheetId="28" r:id="rId24"/>
-    <sheet name="Chat" sheetId="29" r:id="rId25"/>
-    <sheet name="Mylist" sheetId="30" r:id="rId26"/>
-    <sheet name="Forget_Password_Alert" sheetId="31" r:id="rId27"/>
-    <sheet name="List_Tab_Menu_Exclusive" sheetId="34" r:id="rId28"/>
-    <sheet name="News_Default_Kanal" sheetId="36" r:id="rId29"/>
+    <sheet name="Continue_Watching" sheetId="51" r:id="rId2"/>
+    <sheet name="Edit_Profile_Input" sheetId="38" r:id="rId3"/>
+    <sheet name="Edit_Profile_Alert_Named" sheetId="40" r:id="rId4"/>
+    <sheet name="Edit_Profile_Validate_Button" sheetId="44" r:id="rId5"/>
+    <sheet name="Live_Tv_Active_Tab" sheetId="45" r:id="rId6"/>
+    <sheet name="Live_Tv_Tab_Live_And_Catch" sheetId="50" r:id="rId7"/>
+    <sheet name="Homepage_Menu_Tengah" sheetId="46" r:id="rId8"/>
+    <sheet name="Homepage_Menu_Bawah" sheetId="47" r:id="rId9"/>
+    <sheet name="Homepage_Menu_Bawah_Direct" sheetId="48" r:id="rId10"/>
+    <sheet name="Homepage_Menu_Tengah_Direct" sheetId="49" r:id="rId11"/>
+    <sheet name="Edit_Profile_Alert_Phone" sheetId="41" r:id="rId12"/>
+    <sheet name="List_Share" sheetId="35" r:id="rId13"/>
+    <sheet name="Login_Alert_Username" sheetId="20" r:id="rId14"/>
+    <sheet name="Login_Alert_Password" sheetId="21" r:id="rId15"/>
+    <sheet name="Login_Alert_Popup" sheetId="16" r:id="rId16"/>
+    <sheet name="List_Menu_Account_Popup_Login" sheetId="12" r:id="rId17"/>
+    <sheet name="List_Menu_Account_Direct" sheetId="11" r:id="rId18"/>
+    <sheet name="Register_Email_Alert" sheetId="22" r:id="rId19"/>
+    <sheet name="Register_Password1_Alert_Email" sheetId="23" r:id="rId20"/>
+    <sheet name="Register_Password2_Alert_Email" sheetId="24" r:id="rId21"/>
+    <sheet name="Register_Password2_Alert_Phone" sheetId="26" r:id="rId22"/>
+    <sheet name="Register_Password1_Alert_Phone" sheetId="27" r:id="rId23"/>
+    <sheet name="Register_Phone_Alert" sheetId="25" r:id="rId24"/>
+    <sheet name="Register_List_Gender" sheetId="28" r:id="rId25"/>
+    <sheet name="Chat" sheetId="29" r:id="rId26"/>
+    <sheet name="Mylist" sheetId="30" r:id="rId27"/>
+    <sheet name="Forget_Password_Alert" sheetId="31" r:id="rId28"/>
+    <sheet name="List_Tab_Menu_Exclusive" sheetId="34" r:id="rId29"/>
+    <sheet name="News_Default_Kanal" sheetId="36" r:id="rId30"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -52,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="121">
   <si>
     <t>Username</t>
   </si>
@@ -776,8 +777,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -830,7 +831,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
@@ -838,8 +839,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="5.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -858,10 +860,10 @@
         <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C2" t="s">
-        <v>116</v>
+        <v>106</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -869,10 +871,10 @@
         <v>73</v>
       </c>
       <c r="B3" t="s">
-        <v>84</v>
+        <v>107</v>
       </c>
       <c r="C3" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -880,6 +882,91 @@
         <v>74</v>
       </c>
       <c r="B4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" t="s">
         <v>105</v>
       </c>
       <c r="C4" t="s">
@@ -892,7 +979,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -951,7 +1038,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -1014,7 +1101,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -1067,7 +1154,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -1121,7 +1208,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:C3"/>
@@ -1178,7 +1265,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:C4"/>
@@ -1241,7 +1328,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:B5"/>
@@ -1301,7 +1388,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -1367,7 +1454,45 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1419,59 +1544,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.90625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1523,7 +1596,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1575,7 +1648,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1627,7 +1700,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -1690,7 +1763,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
@@ -1720,7 +1793,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -1831,7 +1904,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1869,7 +1942,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -1932,7 +2005,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
@@ -2014,7 +2087,59 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -2065,7 +2190,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -2161,7 +2286,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -2230,7 +2355,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -2290,7 +2415,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -2334,7 +2459,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -2386,7 +2511,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -2450,90 +2575,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="5.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7265625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B6" t="s">
-        <v>109</v>
-      </c>
-      <c r="C6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
optimaized Code and Excecution Testcases
</commit_message>
<xml_diff>
--- a/target/classes/data/data_test.xlsx
+++ b/target/classes/data/data_test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7450" firstSheet="16" activeTab="19"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7450" firstSheet="28" activeTab="29"/>
   </bookViews>
   <sheets>
     <sheet name="Login_Success" sheetId="15" r:id="rId1"/>
@@ -224,9 +224,6 @@
     <t>Nickname</t>
   </si>
   <si>
-    <t>dikakokodikakoko</t>
-  </si>
-  <si>
     <t>rcti</t>
   </si>
   <si>
@@ -456,6 +453,9 @@
   </si>
   <si>
     <t>82290987765</t>
+  </si>
+  <si>
+    <t>akudikakoko</t>
   </si>
 </sst>
 </file>
@@ -885,7 +885,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>51</v>
@@ -893,34 +893,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -945,26 +945,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -989,34 +989,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1040,31 +1040,31 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s">
         <v>51</v>
@@ -1072,18 +1072,18 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -1108,68 +1108,68 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s">
         <v>51</v>
       </c>
       <c r="C4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1193,46 +1193,46 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1266,10 +1266,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>7</v>
@@ -1277,13 +1277,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>45</v>
@@ -1312,50 +1312,50 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1513,8 +1513,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1548,7 +1548,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -2070,26 +2070,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -2102,8 +2102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2131,7 +2131,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -2140,7 +2140,7 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>132</v>
       </c>
       <c r="E2" t="s">
         <v>53</v>
@@ -2148,7 +2148,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -2157,7 +2157,7 @@
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>55</v>
+        <v>132</v>
       </c>
       <c r="E3" t="s">
         <v>53</v>
@@ -2165,7 +2165,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
@@ -2174,7 +2174,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>132</v>
       </c>
       <c r="E4" t="s">
         <v>53</v>
@@ -2182,7 +2182,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>2</v>
@@ -2191,7 +2191,7 @@
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>55</v>
+        <v>132</v>
       </c>
       <c r="E5" t="s">
         <v>53</v>
@@ -2271,7 +2271,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -2279,7 +2279,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
@@ -2287,7 +2287,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
@@ -2295,7 +2295,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B5" t="s">
         <v>12</v>
@@ -2325,66 +2325,66 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -2407,34 +2407,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -2461,21 +2461,21 @@
         <v>42</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -2520,30 +2520,30 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>126</v>
-      </c>
       <c r="E1" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D2" t="s">
         <v>127</v>
       </c>
-      <c r="D2" t="s">
-        <v>128</v>
-      </c>
       <c r="E2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -2576,24 +2576,24 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -2629,10 +2629,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>7</v>
@@ -2640,30 +2640,30 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>2</v>
@@ -2674,16 +2674,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
@@ -2723,40 +2723,40 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>